<commit_message>
Created the DataProvider Util for Excel Data that is used in create job API.
Added the CreateJobAPIExceDataDrivenTest and LoginAPIExcelDataDrivenTest
in testng-datadriven.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/honey/eclipse-workspace/PhoenixTestAutiomationFramework/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001CC321-89EF-6347-8DA6-F35CCBAA3BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDAFBC-8D1B-EB4E-B7EF-C7BF1D663422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{98910CF6-305B-614D-B7BC-4959C139FA39}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20180" activeTab="1" xr2:uid="{98910CF6-305B-614D-B7BC-4959C139FA39}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -51,16 +52,159 @@
   </si>
   <si>
     <t>iameng</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>davinder</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>davin@gmail.com</t>
+  </si>
+  <si>
+    <t>ASDFQW</t>
+  </si>
+  <si>
+    <t>JASKJD</t>
+  </si>
+  <si>
+    <t>WSKJDF</t>
+  </si>
+  <si>
+    <t>N CA</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>2025-08-05T07:00:00.000Z</t>
+  </si>
+  <si>
+    <t>ASDGW34T</t>
+  </si>
+  <si>
+    <t>Vadhav</t>
+  </si>
+  <si>
+    <t>rajv</t>
+  </si>
+  <si>
+    <t>davinder@gmail.com</t>
+  </si>
+  <si>
+    <t>19206239856488</t>
+  </si>
+  <si>
+    <t>19106239856488</t>
+  </si>
+  <si>
+    <t>dasasd@gmail.com</t>
+  </si>
+  <si>
+    <t>davindwe@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,13 +227,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83EA00-B677-D447-9845-48478C9ECA04}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -465,4 +613,301 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64912AD6-134E-F44C-9C41-73BF5BB37701}">
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="35.5" customWidth="1"/>
+    <col min="12" max="12" width="35.6640625" customWidth="1"/>
+    <col min="13" max="13" width="31.1640625" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
+    <col min="15" max="15" width="33.1640625" customWidth="1"/>
+    <col min="16" max="16" width="38.1640625" customWidth="1"/>
+    <col min="17" max="17" width="29.5" customWidth="1"/>
+    <col min="18" max="18" width="26.6640625" customWidth="1"/>
+    <col min="19" max="19" width="24" customWidth="1"/>
+    <col min="20" max="20" width="37.6640625" customWidth="1"/>
+    <col min="21" max="21" width="27" customWidth="1"/>
+    <col min="22" max="22" width="28.33203125" customWidth="1"/>
+    <col min="23" max="23" width="26.1640625" customWidth="1"/>
+    <col min="24" max="24" width="31.6640625" customWidth="1"/>
+    <col min="25" max="25" width="31" customWidth="1"/>
+    <col min="26" max="26" width="18" customWidth="1"/>
+    <col min="27" max="27" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2">
+        <v>8573628492</v>
+      </c>
+      <c r="H2">
+        <v>84756438392</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2">
+        <v>432323</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2">
+        <v>3</v>
+      </c>
+      <c r="Y2">
+        <v>3</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3">
+        <v>8573548492</v>
+      </c>
+      <c r="H3">
+        <v>84755438392</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3">
+        <v>432323</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{45B8D1D8-AE96-6142-BB3A-C179348B496F}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{C0C48126-BAD1-C145-B8E9-225D2AB78166}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>